<commit_message>
Fixed bug in maps in ASSIGNMENT
</commit_message>
<xml_diff>
--- a/ERC_formatted.xlsx
+++ b/ERC_formatted.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samuelsoltys/GitHub/ESC_2023/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{062DBA2E-2825-5E48-8DAB-F155CB8DEA9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B68D87A-9812-7242-8442-249032B569BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25040" yWindow="500" windowWidth="29040" windowHeight="9440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25040" yWindow="500" windowWidth="28900" windowHeight="25920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1_Počet obyvateľov" sheetId="1" r:id="rId1"/>
@@ -561,7 +561,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -663,9 +663,6 @@
     <xf numFmtId="3" fontId="9" fillId="0" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="9" fillId="0" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="9" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="3" fontId="9" fillId="0" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="9" fillId="0" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
@@ -976,8 +973,8 @@
   </sheetPr>
   <dimension ref="A1:M80"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q5" sqref="Q5"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="A53" sqref="A53:M53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -993,7 +990,7 @@
       <c r="B1" s="30">
         <v>2010</v>
       </c>
-      <c r="C1" s="39">
+      <c r="C1" s="29">
         <v>2011</v>
       </c>
       <c r="D1" s="29">
@@ -1023,7 +1020,7 @@
       <c r="L1" s="30">
         <v>2020</v>
       </c>
-      <c r="M1" s="39">
+      <c r="M1" s="29">
         <v>2021</v>
       </c>
     </row>
@@ -1064,7 +1061,7 @@
       <c r="L2" s="33">
         <v>46080</v>
       </c>
-      <c r="M2" s="40">
+      <c r="M2" s="39">
         <v>46432</v>
       </c>
     </row>
@@ -1105,7 +1102,7 @@
       <c r="L3" s="34">
         <v>125179</v>
       </c>
-      <c r="M3" s="40">
+      <c r="M3" s="39">
         <v>125001</v>
       </c>
     </row>
@@ -1146,7 +1143,7 @@
       <c r="L4" s="34">
         <v>76270</v>
       </c>
-      <c r="M4" s="40">
+      <c r="M4" s="39">
         <v>76694</v>
       </c>
     </row>
@@ -1187,7 +1184,7 @@
       <c r="L5" s="34">
         <v>105245</v>
       </c>
-      <c r="M5" s="40">
+      <c r="M5" s="39">
         <v>105154</v>
       </c>
     </row>
@@ -1228,7 +1225,7 @@
       <c r="L6" s="34">
         <v>122729</v>
       </c>
-      <c r="M6" s="40">
+      <c r="M6" s="39">
         <v>122296</v>
       </c>
     </row>
@@ -1269,7 +1266,7 @@
       <c r="L7" s="34">
         <v>78136</v>
       </c>
-      <c r="M7" s="40">
+      <c r="M7" s="39">
         <v>78809</v>
       </c>
     </row>
@@ -1310,7 +1307,7 @@
       <c r="L8" s="34">
         <v>69183</v>
       </c>
-      <c r="M8" s="40">
+      <c r="M8" s="39">
         <v>69623</v>
       </c>
     </row>
@@ -1351,7 +1348,7 @@
       <c r="L9" s="34">
         <v>96715</v>
       </c>
-      <c r="M9" s="40">
+      <c r="M9" s="39">
         <v>99705</v>
       </c>
     </row>
@@ -1392,7 +1389,7 @@
       <c r="L10" s="34">
         <v>124669</v>
       </c>
-      <c r="M10" s="40">
+      <c r="M10" s="39">
         <v>125238</v>
       </c>
     </row>
@@ -1433,7 +1430,7 @@
       <c r="L11" s="34">
         <v>95124</v>
       </c>
-      <c r="M11" s="40">
+      <c r="M11" s="39">
         <v>95027</v>
       </c>
     </row>
@@ -1474,7 +1471,7 @@
       <c r="L12" s="34">
         <v>44015</v>
       </c>
-      <c r="M12" s="40">
+      <c r="M12" s="39">
         <v>43769</v>
       </c>
     </row>
@@ -1515,7 +1512,7 @@
       <c r="L13" s="34">
         <v>63032</v>
       </c>
-      <c r="M13" s="40">
+      <c r="M13" s="39">
         <v>62662</v>
       </c>
     </row>
@@ -1556,7 +1553,7 @@
       <c r="L14" s="34">
         <v>59749</v>
       </c>
-      <c r="M14" s="40">
+      <c r="M14" s="39">
         <v>59347</v>
       </c>
     </row>
@@ -1597,7 +1594,7 @@
       <c r="L15" s="34">
         <v>47525</v>
       </c>
-      <c r="M15" s="40">
+      <c r="M15" s="39">
         <v>47313</v>
       </c>
     </row>
@@ -1638,7 +1635,7 @@
       <c r="L16" s="34">
         <v>131894</v>
       </c>
-      <c r="M16" s="40">
+      <c r="M16" s="39">
         <v>131940</v>
       </c>
     </row>
@@ -1679,7 +1676,7 @@
       <c r="L17" s="34">
         <v>35967</v>
       </c>
-      <c r="M17" s="40">
+      <c r="M17" s="39">
         <v>35658</v>
       </c>
     </row>
@@ -1720,7 +1717,7 @@
       <c r="L18" s="34">
         <v>58058</v>
       </c>
-      <c r="M18" s="40">
+      <c r="M18" s="39">
         <v>57511</v>
       </c>
     </row>
@@ -1761,7 +1758,7 @@
       <c r="L19" s="34">
         <v>25678</v>
       </c>
-      <c r="M19" s="40">
+      <c r="M19" s="39">
         <v>25363</v>
       </c>
     </row>
@@ -1802,7 +1799,7 @@
       <c r="L20" s="34">
         <v>61840</v>
       </c>
-      <c r="M20" s="40">
+      <c r="M20" s="39">
         <v>61512</v>
       </c>
     </row>
@@ -1843,7 +1840,7 @@
       <c r="L21" s="34">
         <v>44515</v>
       </c>
-      <c r="M21" s="40">
+      <c r="M21" s="39">
         <v>44179</v>
       </c>
     </row>
@@ -1884,7 +1881,7 @@
       <c r="L22" s="34">
         <v>61617</v>
       </c>
-      <c r="M22" s="40">
+      <c r="M22" s="39">
         <v>61211</v>
       </c>
     </row>
@@ -1925,7 +1922,7 @@
       <c r="L23" s="34">
         <v>131693</v>
       </c>
-      <c r="M23" s="40">
+      <c r="M23" s="39">
         <v>130616</v>
       </c>
     </row>
@@ -1966,7 +1963,7 @@
       <c r="L24" s="34">
         <v>44319</v>
       </c>
-      <c r="M24" s="40">
+      <c r="M24" s="39">
         <v>44133</v>
       </c>
     </row>
@@ -2007,7 +2004,7 @@
       <c r="L25" s="34">
         <v>113777</v>
       </c>
-      <c r="M25" s="40">
+      <c r="M25" s="39">
         <v>113516</v>
       </c>
     </row>
@@ -2048,7 +2045,7 @@
       <c r="L26" s="34">
         <v>100952</v>
       </c>
-      <c r="M26" s="40">
+      <c r="M26" s="39">
         <v>100212</v>
       </c>
     </row>
@@ -2089,7 +2086,7 @@
       <c r="L27" s="34">
         <v>110469</v>
       </c>
-      <c r="M27" s="40">
+      <c r="M27" s="39">
         <v>109588</v>
       </c>
     </row>
@@ -2130,7 +2127,7 @@
       <c r="L28" s="34">
         <v>164788</v>
       </c>
-      <c r="M28" s="40">
+      <c r="M28" s="39">
         <v>164580</v>
       </c>
     </row>
@@ -2171,7 +2168,7 @@
       <c r="L29" s="34">
         <v>138168</v>
       </c>
-      <c r="M29" s="40">
+      <c r="M29" s="39">
         <v>137001</v>
       </c>
     </row>
@@ -2212,7 +2209,7 @@
       <c r="L30" s="34">
         <v>51477</v>
       </c>
-      <c r="M30" s="40">
+      <c r="M30" s="39">
         <v>50972</v>
       </c>
     </row>
@@ -2253,7 +2250,7 @@
       <c r="L31" s="34">
         <v>70877</v>
       </c>
-      <c r="M31" s="40">
+      <c r="M31" s="39">
         <v>70313</v>
       </c>
     </row>
@@ -2294,7 +2291,7 @@
       <c r="L32" s="34">
         <v>41169</v>
       </c>
-      <c r="M32" s="40">
+      <c r="M32" s="39">
         <v>40881</v>
       </c>
     </row>
@@ -2335,7 +2332,7 @@
       <c r="L33" s="34">
         <v>31154</v>
       </c>
-      <c r="M33" s="40">
+      <c r="M33" s="39">
         <v>31163</v>
       </c>
     </row>
@@ -2376,7 +2373,7 @@
       <c r="L34" s="34">
         <v>88642</v>
       </c>
-      <c r="M34" s="40">
+      <c r="M34" s="39">
         <v>87969</v>
       </c>
     </row>
@@ -2417,7 +2414,7 @@
       <c r="L35" s="34">
         <v>39026</v>
       </c>
-      <c r="M35" s="40">
+      <c r="M35" s="39">
         <v>38937</v>
       </c>
     </row>
@@ -2458,7 +2455,7 @@
       <c r="L36" s="34">
         <v>32699</v>
       </c>
-      <c r="M36" s="40">
+      <c r="M36" s="39">
         <v>32654</v>
       </c>
     </row>
@@ -2499,7 +2496,7 @@
       <c r="L37" s="34">
         <v>71935</v>
       </c>
-      <c r="M37" s="40">
+      <c r="M37" s="39">
         <v>71685</v>
       </c>
     </row>
@@ -2540,7 +2537,7 @@
       <c r="L38" s="34">
         <v>94376</v>
       </c>
-      <c r="M38" s="40">
+      <c r="M38" s="39">
         <v>93816</v>
       </c>
     </row>
@@ -2581,7 +2578,7 @@
       <c r="L39" s="34">
         <v>63200</v>
       </c>
-      <c r="M39" s="40">
+      <c r="M39" s="39">
         <v>63563</v>
       </c>
     </row>
@@ -2622,7 +2619,7 @@
       <c r="L40" s="34">
         <v>57392</v>
       </c>
-      <c r="M40" s="40">
+      <c r="M40" s="39">
         <v>57036</v>
       </c>
     </row>
@@ -2663,500 +2660,500 @@
       <c r="L41" s="34">
         <v>15956</v>
       </c>
-      <c r="M41" s="40">
+      <c r="M41" s="39">
         <v>15848</v>
       </c>
     </row>
     <row r="42" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="B42" s="34">
-        <v>45666</v>
+        <v>35750</v>
       </c>
       <c r="C42" s="37">
-        <v>45496</v>
+        <v>35908</v>
       </c>
       <c r="D42" s="12">
-        <v>45280</v>
+        <v>36010</v>
       </c>
       <c r="E42" s="4">
-        <v>45086</v>
+        <v>36037</v>
       </c>
       <c r="F42" s="12">
-        <v>44826</v>
+        <v>36066</v>
       </c>
       <c r="G42" s="4">
-        <v>44489</v>
+        <v>35995</v>
       </c>
       <c r="H42" s="12">
-        <v>44212</v>
+        <v>36053</v>
       </c>
       <c r="I42" s="4">
-        <v>43992</v>
+        <v>36104</v>
       </c>
       <c r="J42" s="12">
-        <v>43683</v>
+        <v>36157</v>
       </c>
       <c r="K42" s="4">
-        <v>43263</v>
+        <v>36203</v>
       </c>
       <c r="L42" s="34">
-        <v>41998</v>
-      </c>
-      <c r="M42" s="40">
-        <v>41605</v>
+        <v>35856</v>
+      </c>
+      <c r="M42" s="39">
+        <v>35802</v>
       </c>
     </row>
     <row r="43" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B43" s="34">
-        <v>35750</v>
+        <v>153858</v>
       </c>
       <c r="C43" s="37">
-        <v>35908</v>
+        <v>154596</v>
       </c>
       <c r="D43" s="12">
-        <v>36010</v>
+        <v>155084</v>
       </c>
       <c r="E43" s="4">
-        <v>36037</v>
+        <v>155574</v>
       </c>
       <c r="F43" s="12">
-        <v>36066</v>
+        <v>155989</v>
       </c>
       <c r="G43" s="4">
-        <v>35995</v>
+        <v>156411</v>
       </c>
       <c r="H43" s="12">
-        <v>36053</v>
+        <v>156826</v>
       </c>
       <c r="I43" s="4">
-        <v>36104</v>
+        <v>157281</v>
       </c>
       <c r="J43" s="12">
-        <v>36157</v>
+        <v>157807</v>
       </c>
       <c r="K43" s="4">
-        <v>36203</v>
+        <v>158279</v>
       </c>
       <c r="L43" s="34">
-        <v>35856</v>
-      </c>
-      <c r="M43" s="40">
-        <v>35802</v>
+        <v>161377</v>
+      </c>
+      <c r="M43" s="39">
+        <v>161052</v>
       </c>
     </row>
     <row r="44" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B44" s="34">
-        <v>153858</v>
+        <v>111226</v>
       </c>
       <c r="C44" s="37">
-        <v>154596</v>
+        <v>111180</v>
       </c>
       <c r="D44" s="12">
-        <v>155084</v>
+        <v>111148</v>
       </c>
       <c r="E44" s="4">
-        <v>155574</v>
+        <v>111112</v>
       </c>
       <c r="F44" s="12">
-        <v>155989</v>
+        <v>111018</v>
       </c>
       <c r="G44" s="4">
-        <v>156411</v>
+        <v>110920</v>
       </c>
       <c r="H44" s="12">
-        <v>156826</v>
+        <v>110925</v>
       </c>
       <c r="I44" s="4">
-        <v>157281</v>
+        <v>110931</v>
       </c>
       <c r="J44" s="12">
-        <v>157807</v>
+        <v>110941</v>
       </c>
       <c r="K44" s="4">
-        <v>158279</v>
+        <v>110716</v>
       </c>
       <c r="L44" s="34">
-        <v>161377</v>
-      </c>
-      <c r="M44" s="40">
-        <v>161052</v>
+        <v>108730</v>
+      </c>
+      <c r="M44" s="39">
+        <v>108120</v>
       </c>
     </row>
     <row r="45" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B45" s="34">
-        <v>111226</v>
+        <v>16640</v>
       </c>
       <c r="C45" s="37">
-        <v>111180</v>
+        <v>16580</v>
       </c>
       <c r="D45" s="12">
-        <v>111148</v>
+        <v>16509</v>
       </c>
       <c r="E45" s="4">
-        <v>111112</v>
+        <v>16414</v>
       </c>
       <c r="F45" s="12">
-        <v>111018</v>
+        <v>16367</v>
       </c>
       <c r="G45" s="4">
-        <v>110920</v>
+        <v>16314</v>
       </c>
       <c r="H45" s="12">
-        <v>110925</v>
+        <v>16260</v>
       </c>
       <c r="I45" s="4">
-        <v>110931</v>
+        <v>16165</v>
       </c>
       <c r="J45" s="12">
-        <v>110941</v>
+        <v>16103</v>
       </c>
       <c r="K45" s="4">
-        <v>110716</v>
+        <v>16069</v>
       </c>
       <c r="L45" s="34">
-        <v>108730</v>
-      </c>
-      <c r="M45" s="40">
-        <v>108120</v>
+        <v>15649</v>
+      </c>
+      <c r="M45" s="39">
+        <v>15551</v>
       </c>
     </row>
     <row r="46" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B46" s="34">
-        <v>16640</v>
+        <v>64250</v>
       </c>
       <c r="C46" s="37">
-        <v>16580</v>
+        <v>64076</v>
       </c>
       <c r="D46" s="12">
-        <v>16509</v>
+        <v>63696</v>
       </c>
       <c r="E46" s="4">
-        <v>16414</v>
+        <v>63326</v>
       </c>
       <c r="F46" s="12">
-        <v>16367</v>
+        <v>62971</v>
       </c>
       <c r="G46" s="4">
-        <v>16314</v>
+        <v>62616</v>
       </c>
       <c r="H46" s="12">
-        <v>16260</v>
+        <v>62298</v>
       </c>
       <c r="I46" s="4">
-        <v>16165</v>
+        <v>61959</v>
       </c>
       <c r="J46" s="12">
-        <v>16103</v>
+        <v>61630</v>
       </c>
       <c r="K46" s="4">
-        <v>16069</v>
+        <v>61269</v>
       </c>
       <c r="L46" s="34">
-        <v>15649</v>
-      </c>
-      <c r="M46" s="40">
-        <v>15551</v>
+        <v>59446</v>
+      </c>
+      <c r="M46" s="39">
+        <v>58965</v>
       </c>
     </row>
     <row r="47" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B47" s="34">
-        <v>64250</v>
+        <v>32931</v>
       </c>
       <c r="C47" s="37">
-        <v>64076</v>
+        <v>32941</v>
       </c>
       <c r="D47" s="12">
-        <v>63696</v>
+        <v>32871</v>
       </c>
       <c r="E47" s="4">
-        <v>63326</v>
+        <v>32722</v>
       </c>
       <c r="F47" s="12">
-        <v>62971</v>
+        <v>32632</v>
       </c>
       <c r="G47" s="4">
-        <v>62616</v>
+        <v>32505</v>
       </c>
       <c r="H47" s="12">
-        <v>62298</v>
+        <v>32418</v>
       </c>
       <c r="I47" s="4">
-        <v>61959</v>
+        <v>32270</v>
       </c>
       <c r="J47" s="12">
-        <v>61630</v>
+        <v>32135</v>
       </c>
       <c r="K47" s="4">
-        <v>61269</v>
+        <v>31967</v>
       </c>
       <c r="L47" s="34">
-        <v>59446</v>
-      </c>
-      <c r="M47" s="40">
-        <v>58965</v>
+        <v>31034</v>
+      </c>
+      <c r="M47" s="39">
+        <v>30854</v>
       </c>
     </row>
     <row r="48" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B48" s="34">
-        <v>32931</v>
+        <v>22970</v>
       </c>
       <c r="C48" s="37">
-        <v>32941</v>
+        <v>22909</v>
       </c>
       <c r="D48" s="12">
-        <v>32871</v>
+        <v>22779</v>
       </c>
       <c r="E48" s="4">
-        <v>32722</v>
+        <v>22710</v>
       </c>
       <c r="F48" s="12">
-        <v>32632</v>
+        <v>22636</v>
       </c>
       <c r="G48" s="4">
-        <v>32505</v>
+        <v>22530</v>
       </c>
       <c r="H48" s="12">
-        <v>32418</v>
+        <v>22421</v>
       </c>
       <c r="I48" s="4">
-        <v>32270</v>
+        <v>22299</v>
       </c>
       <c r="J48" s="12">
-        <v>32135</v>
+        <v>22225</v>
       </c>
       <c r="K48" s="4">
-        <v>31967</v>
+        <v>22139</v>
       </c>
       <c r="L48" s="34">
-        <v>31034</v>
-      </c>
-      <c r="M48" s="40">
-        <v>30854</v>
+        <v>21517</v>
+      </c>
+      <c r="M48" s="39">
+        <v>21366</v>
       </c>
     </row>
     <row r="49" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B49" s="34">
-        <v>22970</v>
+        <v>74875</v>
       </c>
       <c r="C49" s="37">
-        <v>22909</v>
+        <v>74844</v>
       </c>
       <c r="D49" s="12">
-        <v>22779</v>
+        <v>74681</v>
       </c>
       <c r="E49" s="4">
-        <v>22710</v>
+        <v>74548</v>
       </c>
       <c r="F49" s="12">
-        <v>22636</v>
+        <v>74401</v>
       </c>
       <c r="G49" s="4">
-        <v>22530</v>
+        <v>74106</v>
       </c>
       <c r="H49" s="12">
-        <v>22421</v>
+        <v>74045</v>
       </c>
       <c r="I49" s="4">
-        <v>22299</v>
+        <v>73849</v>
       </c>
       <c r="J49" s="12">
-        <v>22225</v>
+        <v>73590</v>
       </c>
       <c r="K49" s="4">
-        <v>22139</v>
+        <v>73342</v>
       </c>
       <c r="L49" s="34">
-        <v>21517</v>
-      </c>
-      <c r="M49" s="40">
-        <v>21366</v>
+        <v>70422</v>
+      </c>
+      <c r="M49" s="39">
+        <v>69788</v>
       </c>
     </row>
     <row r="50" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B50" s="34">
-        <v>74875</v>
+        <v>22586</v>
       </c>
       <c r="C50" s="37">
-        <v>74844</v>
+        <v>22480</v>
       </c>
       <c r="D50" s="12">
-        <v>74681</v>
+        <v>22400</v>
       </c>
       <c r="E50" s="4">
-        <v>74548</v>
+        <v>22226</v>
       </c>
       <c r="F50" s="12">
-        <v>74401</v>
+        <v>22074</v>
       </c>
       <c r="G50" s="4">
-        <v>74106</v>
+        <v>21930</v>
       </c>
       <c r="H50" s="12">
-        <v>74045</v>
+        <v>21767</v>
       </c>
       <c r="I50" s="4">
-        <v>73849</v>
+        <v>21644</v>
       </c>
       <c r="J50" s="12">
-        <v>73590</v>
+        <v>21545</v>
       </c>
       <c r="K50" s="4">
-        <v>73342</v>
+        <v>21397</v>
       </c>
       <c r="L50" s="34">
-        <v>70422</v>
-      </c>
-      <c r="M50" s="40">
-        <v>69788</v>
+        <v>20634</v>
+      </c>
+      <c r="M50" s="39">
+        <v>20427</v>
       </c>
     </row>
     <row r="51" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B51" s="34">
-        <v>22586</v>
+        <v>40428</v>
       </c>
       <c r="C51" s="37">
-        <v>22480</v>
+        <v>40419</v>
       </c>
       <c r="D51" s="12">
-        <v>22400</v>
+        <v>40326</v>
       </c>
       <c r="E51" s="4">
-        <v>22226</v>
+        <v>40237</v>
       </c>
       <c r="F51" s="12">
-        <v>22074</v>
+        <v>40205</v>
       </c>
       <c r="G51" s="4">
-        <v>21930</v>
+        <v>40124</v>
       </c>
       <c r="H51" s="12">
-        <v>21767</v>
+        <v>40052</v>
       </c>
       <c r="I51" s="4">
-        <v>21644</v>
+        <v>39971</v>
       </c>
       <c r="J51" s="12">
-        <v>21545</v>
+        <v>39736</v>
       </c>
       <c r="K51" s="4">
-        <v>21397</v>
+        <v>39537</v>
       </c>
       <c r="L51" s="34">
-        <v>20634</v>
-      </c>
-      <c r="M51" s="40">
-        <v>20427</v>
+        <v>38669</v>
+      </c>
+      <c r="M51" s="39">
+        <v>38242</v>
       </c>
     </row>
     <row r="52" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B52" s="34">
-        <v>40428</v>
+        <v>84947</v>
       </c>
       <c r="C52" s="37">
-        <v>40419</v>
+        <v>84867</v>
       </c>
       <c r="D52" s="12">
-        <v>40326</v>
+        <v>84837</v>
       </c>
       <c r="E52" s="4">
-        <v>40237</v>
+        <v>84764</v>
       </c>
       <c r="F52" s="12">
-        <v>40205</v>
+        <v>84752</v>
       </c>
       <c r="G52" s="4">
-        <v>40124</v>
+        <v>84577</v>
       </c>
       <c r="H52" s="12">
-        <v>40052</v>
+        <v>84518</v>
       </c>
       <c r="I52" s="4">
-        <v>39971</v>
+        <v>84331</v>
       </c>
       <c r="J52" s="12">
-        <v>39736</v>
+        <v>84270</v>
       </c>
       <c r="K52" s="4">
-        <v>39537</v>
+        <v>84048</v>
       </c>
       <c r="L52" s="34">
-        <v>38669</v>
-      </c>
-      <c r="M52" s="40">
-        <v>38242</v>
+        <v>80666</v>
+      </c>
+      <c r="M52" s="39">
+        <v>80359</v>
       </c>
     </row>
     <row r="53" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B53" s="34">
-        <v>84947</v>
+        <v>45666</v>
       </c>
       <c r="C53" s="37">
-        <v>84867</v>
+        <v>45496</v>
       </c>
       <c r="D53" s="12">
-        <v>84837</v>
+        <v>45280</v>
       </c>
       <c r="E53" s="4">
-        <v>84764</v>
+        <v>45086</v>
       </c>
       <c r="F53" s="12">
-        <v>84752</v>
+        <v>44826</v>
       </c>
       <c r="G53" s="4">
-        <v>84577</v>
+        <v>44489</v>
       </c>
       <c r="H53" s="12">
-        <v>84518</v>
+        <v>44212</v>
       </c>
       <c r="I53" s="4">
-        <v>84331</v>
+        <v>43992</v>
       </c>
       <c r="J53" s="12">
-        <v>84270</v>
+        <v>43683</v>
       </c>
       <c r="K53" s="4">
-        <v>84048</v>
+        <v>43263</v>
       </c>
       <c r="L53" s="34">
-        <v>80666</v>
-      </c>
-      <c r="M53" s="40">
-        <v>80359</v>
+        <v>41998</v>
+      </c>
+      <c r="M53" s="39">
+        <v>41605</v>
       </c>
     </row>
     <row r="54" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -3196,7 +3193,7 @@
       <c r="L54" s="34">
         <v>66750</v>
       </c>
-      <c r="M54" s="40">
+      <c r="M54" s="39">
         <v>66294</v>
       </c>
     </row>
@@ -3237,7 +3234,7 @@
       <c r="L55" s="34">
         <v>25242</v>
       </c>
-      <c r="M55" s="40">
+      <c r="M55" s="39">
         <v>24991</v>
       </c>
     </row>
@@ -3278,7 +3275,7 @@
       <c r="L56" s="34">
         <v>44844</v>
       </c>
-      <c r="M56" s="40">
+      <c r="M56" s="39">
         <v>44424</v>
       </c>
     </row>
@@ -3319,7 +3316,7 @@
       <c r="L57" s="34">
         <v>76012</v>
       </c>
-      <c r="M57" s="40">
+      <c r="M57" s="39">
         <v>75786</v>
       </c>
     </row>
@@ -3360,7 +3357,7 @@
       <c r="L58" s="34">
         <v>60126</v>
       </c>
-      <c r="M58" s="40">
+      <c r="M58" s="39">
         <v>59535</v>
       </c>
     </row>
@@ -3401,7 +3398,7 @@
       <c r="L59" s="34">
         <v>73685</v>
       </c>
-      <c r="M59" s="40">
+      <c r="M59" s="39">
         <v>74232</v>
       </c>
     </row>
@@ -3442,7 +3439,7 @@
       <c r="L60" s="34">
         <v>33107</v>
       </c>
-      <c r="M60" s="40">
+      <c r="M60" s="39">
         <v>33127</v>
       </c>
     </row>
@@ -3483,7 +3480,7 @@
       <c r="L61" s="34">
         <v>11056</v>
       </c>
-      <c r="M61" s="40">
+      <c r="M61" s="39">
         <v>10870</v>
       </c>
     </row>
@@ -3524,7 +3521,7 @@
       <c r="L62" s="34">
         <v>102744</v>
       </c>
-      <c r="M62" s="40">
+      <c r="M62" s="39">
         <v>102469</v>
       </c>
     </row>
@@ -3565,7 +3562,7 @@
       <c r="L63" s="34">
         <v>172804</v>
       </c>
-      <c r="M63" s="40">
+      <c r="M63" s="39">
         <v>173187</v>
       </c>
     </row>
@@ -3606,7 +3603,7 @@
       <c r="L64" s="34">
         <v>60389</v>
       </c>
-      <c r="M64" s="40">
+      <c r="M64" s="39">
         <v>60607</v>
       </c>
     </row>
@@ -3647,7 +3644,7 @@
       <c r="L65" s="34">
         <v>35125</v>
       </c>
-      <c r="M65" s="40">
+      <c r="M65" s="39">
         <v>34655</v>
       </c>
     </row>
@@ -3688,7 +3685,7 @@
       <c r="L66" s="34">
         <v>52968</v>
       </c>
-      <c r="M66" s="40">
+      <c r="M66" s="39">
         <v>52867</v>
       </c>
     </row>
@@ -3729,7 +3726,7 @@
       <c r="L67" s="34">
         <v>19878</v>
       </c>
-      <c r="M67" s="40">
+      <c r="M67" s="39">
         <v>19744</v>
       </c>
     </row>
@@ -3770,7 +3767,7 @@
       <c r="L68" s="34">
         <v>31611</v>
       </c>
-      <c r="M68" s="40">
+      <c r="M68" s="39">
         <v>31397</v>
       </c>
     </row>
@@ -3811,7 +3808,7 @@
       <c r="L69" s="34">
         <v>79426</v>
       </c>
-      <c r="M69" s="40">
+      <c r="M69" s="39">
         <v>79181</v>
       </c>
     </row>
@@ -3852,7 +3849,7 @@
       <c r="L70" s="34">
         <v>31698</v>
       </c>
-      <c r="M70" s="40">
+      <c r="M70" s="39">
         <v>31668</v>
       </c>
     </row>
@@ -3893,7 +3890,7 @@
       <c r="L71" s="34">
         <v>64453</v>
       </c>
-      <c r="M71" s="40">
+      <c r="M71" s="39">
         <v>63904</v>
       </c>
     </row>
@@ -3934,7 +3931,7 @@
       <c r="L72" s="34">
         <v>79437</v>
       </c>
-      <c r="M72" s="40">
+      <c r="M72" s="39">
         <v>79034</v>
       </c>
     </row>
@@ -3975,7 +3972,7 @@
       <c r="L73" s="34">
         <v>28135</v>
       </c>
-      <c r="M73" s="40">
+      <c r="M73" s="39">
         <v>27924</v>
       </c>
     </row>
@@ -4016,7 +4013,7 @@
       <c r="L74" s="34">
         <v>57015</v>
       </c>
-      <c r="M74" s="40">
+      <c r="M74" s="39">
         <v>56596</v>
       </c>
     </row>
@@ -4057,7 +4054,7 @@
       <c r="L75" s="34">
         <v>128346</v>
       </c>
-      <c r="M75" s="40">
+      <c r="M75" s="39">
         <v>129237</v>
       </c>
     </row>
@@ -4098,7 +4095,7 @@
       <c r="L76" s="34">
         <v>108954</v>
       </c>
-      <c r="M76" s="40">
+      <c r="M76" s="39">
         <v>108520</v>
       </c>
     </row>
@@ -4139,7 +4136,7 @@
       <c r="L77" s="34">
         <v>59345</v>
       </c>
-      <c r="M77" s="40">
+      <c r="M77" s="39">
         <v>58995</v>
       </c>
     </row>
@@ -4180,7 +4177,7 @@
       <c r="L78" s="34">
         <v>22440</v>
       </c>
-      <c r="M78" s="40">
+      <c r="M78" s="39">
         <v>22377</v>
       </c>
     </row>
@@ -4221,7 +4218,7 @@
       <c r="L79" s="34">
         <v>98706</v>
       </c>
-      <c r="M79" s="40">
+      <c r="M79" s="39">
         <v>98656</v>
       </c>
     </row>
@@ -4262,7 +4259,7 @@
       <c r="L80" s="35">
         <v>103687</v>
       </c>
-      <c r="M80" s="41">
+      <c r="M80" s="40">
         <v>103377</v>
       </c>
     </row>
@@ -10881,7 +10878,9 @@
   </sheetPr>
   <dimension ref="A1:M80"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A53" sqref="A53:M53"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -12572,494 +12571,494 @@
     </row>
     <row r="42" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="B42" s="12">
-        <v>415</v>
+        <v>461</v>
       </c>
       <c r="C42" s="4">
-        <v>409</v>
+        <v>461</v>
       </c>
       <c r="D42" s="12">
-        <v>389</v>
+        <v>439</v>
       </c>
       <c r="E42" s="4">
-        <v>383</v>
+        <v>375</v>
       </c>
       <c r="F42" s="12">
-        <v>400</v>
+        <v>414</v>
       </c>
       <c r="G42" s="4">
         <v>370</v>
       </c>
       <c r="H42" s="12">
-        <v>393</v>
+        <v>417</v>
       </c>
       <c r="I42" s="4">
-        <v>355</v>
+        <v>428</v>
       </c>
       <c r="J42" s="12">
-        <v>378</v>
+        <v>416</v>
       </c>
       <c r="K42" s="4">
-        <v>362</v>
+        <v>439</v>
       </c>
       <c r="L42" s="12">
-        <v>349</v>
+        <v>422</v>
       </c>
       <c r="M42" s="4">
-        <v>333</v>
+        <v>403</v>
       </c>
     </row>
     <row r="43" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B43" s="12">
-        <v>461</v>
+        <v>1691</v>
       </c>
       <c r="C43" s="4">
-        <v>461</v>
+        <v>1790</v>
       </c>
       <c r="D43" s="12">
-        <v>439</v>
+        <v>1685</v>
       </c>
       <c r="E43" s="4">
-        <v>375</v>
+        <v>1637</v>
       </c>
       <c r="F43" s="12">
-        <v>414</v>
+        <v>1573</v>
       </c>
       <c r="G43" s="4">
-        <v>370</v>
+        <v>1700</v>
       </c>
       <c r="H43" s="12">
-        <v>417</v>
+        <v>1736</v>
       </c>
       <c r="I43" s="4">
-        <v>428</v>
+        <v>1739</v>
       </c>
       <c r="J43" s="12">
-        <v>416</v>
+        <v>1722</v>
       </c>
       <c r="K43" s="4">
-        <v>439</v>
+        <v>1735</v>
       </c>
       <c r="L43" s="12">
-        <v>422</v>
+        <v>1695</v>
       </c>
       <c r="M43" s="4">
-        <v>403</v>
+        <v>1654</v>
       </c>
     </row>
     <row r="44" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B44" s="12">
-        <v>1691</v>
+        <v>1095</v>
       </c>
       <c r="C44" s="4">
-        <v>1790</v>
+        <v>1093</v>
       </c>
       <c r="D44" s="12">
-        <v>1685</v>
+        <v>1005</v>
       </c>
       <c r="E44" s="4">
-        <v>1637</v>
+        <v>995</v>
       </c>
       <c r="F44" s="12">
-        <v>1573</v>
+        <v>1006</v>
       </c>
       <c r="G44" s="4">
-        <v>1700</v>
+        <v>1024</v>
       </c>
       <c r="H44" s="12">
-        <v>1736</v>
+        <v>1038</v>
       </c>
       <c r="I44" s="4">
-        <v>1739</v>
+        <v>1015</v>
       </c>
       <c r="J44" s="12">
-        <v>1722</v>
+        <v>1073</v>
       </c>
       <c r="K44" s="4">
-        <v>1735</v>
+        <v>1041</v>
       </c>
       <c r="L44" s="12">
-        <v>1695</v>
+        <v>1025</v>
       </c>
       <c r="M44" s="4">
-        <v>1654</v>
+        <v>990</v>
       </c>
     </row>
     <row r="45" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B45" s="12">
-        <v>1095</v>
+        <v>182</v>
       </c>
       <c r="C45" s="4">
-        <v>1093</v>
+        <v>159</v>
       </c>
       <c r="D45" s="12">
-        <v>1005</v>
+        <v>131</v>
       </c>
       <c r="E45" s="4">
-        <v>995</v>
+        <v>136</v>
       </c>
       <c r="F45" s="12">
-        <v>1006</v>
+        <v>131</v>
       </c>
       <c r="G45" s="4">
-        <v>1024</v>
+        <v>134</v>
       </c>
       <c r="H45" s="12">
-        <v>1038</v>
+        <v>120</v>
       </c>
       <c r="I45" s="4">
-        <v>1015</v>
+        <v>156</v>
       </c>
       <c r="J45" s="12">
-        <v>1073</v>
+        <v>159</v>
       </c>
       <c r="K45" s="4">
-        <v>1041</v>
+        <v>141</v>
       </c>
       <c r="L45" s="12">
-        <v>1025</v>
+        <v>165</v>
       </c>
       <c r="M45" s="4">
-        <v>990</v>
+        <v>155</v>
       </c>
     </row>
     <row r="46" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B46" s="12">
-        <v>182</v>
+        <v>639</v>
       </c>
       <c r="C46" s="4">
-        <v>159</v>
+        <v>662</v>
       </c>
       <c r="D46" s="12">
-        <v>131</v>
+        <v>559</v>
       </c>
       <c r="E46" s="4">
-        <v>136</v>
+        <v>605</v>
       </c>
       <c r="F46" s="12">
-        <v>131</v>
+        <v>555</v>
       </c>
       <c r="G46" s="4">
-        <v>134</v>
+        <v>537</v>
       </c>
       <c r="H46" s="12">
-        <v>120</v>
+        <v>566</v>
       </c>
       <c r="I46" s="4">
-        <v>156</v>
+        <v>591</v>
       </c>
       <c r="J46" s="12">
-        <v>159</v>
+        <v>575</v>
       </c>
       <c r="K46" s="4">
-        <v>141</v>
+        <v>552</v>
       </c>
       <c r="L46" s="12">
-        <v>165</v>
+        <v>571</v>
       </c>
       <c r="M46" s="4">
-        <v>155</v>
+        <v>554</v>
       </c>
     </row>
     <row r="47" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B47" s="12">
-        <v>639</v>
+        <v>303</v>
       </c>
       <c r="C47" s="4">
-        <v>662</v>
+        <v>328</v>
       </c>
       <c r="D47" s="12">
-        <v>559</v>
+        <v>300</v>
       </c>
       <c r="E47" s="4">
-        <v>605</v>
+        <v>277</v>
       </c>
       <c r="F47" s="12">
-        <v>555</v>
+        <v>254</v>
       </c>
       <c r="G47" s="4">
-        <v>537</v>
+        <v>270</v>
       </c>
       <c r="H47" s="12">
-        <v>566</v>
+        <v>284</v>
       </c>
       <c r="I47" s="4">
-        <v>591</v>
+        <v>295</v>
       </c>
       <c r="J47" s="12">
-        <v>575</v>
+        <v>277</v>
       </c>
       <c r="K47" s="4">
-        <v>552</v>
+        <v>278</v>
       </c>
       <c r="L47" s="12">
-        <v>571</v>
+        <v>265</v>
       </c>
       <c r="M47" s="4">
-        <v>554</v>
+        <v>288</v>
       </c>
     </row>
     <row r="48" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B48" s="12">
-        <v>303</v>
+        <v>249</v>
       </c>
       <c r="C48" s="4">
-        <v>328</v>
+        <v>233</v>
       </c>
       <c r="D48" s="12">
-        <v>300</v>
+        <v>188</v>
       </c>
       <c r="E48" s="4">
-        <v>277</v>
+        <v>215</v>
       </c>
       <c r="F48" s="12">
-        <v>254</v>
+        <v>201</v>
       </c>
       <c r="G48" s="4">
-        <v>270</v>
+        <v>215</v>
       </c>
       <c r="H48" s="12">
-        <v>284</v>
+        <v>249</v>
       </c>
       <c r="I48" s="4">
-        <v>295</v>
+        <v>221</v>
       </c>
       <c r="J48" s="12">
-        <v>277</v>
+        <v>249</v>
       </c>
       <c r="K48" s="4">
-        <v>278</v>
+        <v>245</v>
       </c>
       <c r="L48" s="12">
-        <v>265</v>
+        <v>239</v>
       </c>
       <c r="M48" s="4">
-        <v>288</v>
+        <v>220</v>
       </c>
     </row>
     <row r="49" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B49" s="12">
-        <v>249</v>
+        <v>832</v>
       </c>
       <c r="C49" s="4">
-        <v>233</v>
+        <v>815</v>
       </c>
       <c r="D49" s="12">
-        <v>188</v>
+        <v>698</v>
       </c>
       <c r="E49" s="4">
-        <v>215</v>
+        <v>701</v>
       </c>
       <c r="F49" s="12">
-        <v>201</v>
+        <v>706</v>
       </c>
       <c r="G49" s="4">
-        <v>215</v>
+        <v>655</v>
       </c>
       <c r="H49" s="12">
-        <v>249</v>
+        <v>734</v>
       </c>
       <c r="I49" s="4">
-        <v>221</v>
+        <v>719</v>
       </c>
       <c r="J49" s="12">
-        <v>249</v>
+        <v>654</v>
       </c>
       <c r="K49" s="4">
-        <v>245</v>
+        <v>622</v>
       </c>
       <c r="L49" s="12">
-        <v>239</v>
+        <v>640</v>
       </c>
       <c r="M49" s="4">
-        <v>220</v>
+        <v>634</v>
       </c>
     </row>
     <row r="50" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B50" s="12">
-        <v>832</v>
+        <v>214</v>
       </c>
       <c r="C50" s="4">
-        <v>815</v>
+        <v>200</v>
       </c>
       <c r="D50" s="12">
-        <v>698</v>
+        <v>173</v>
       </c>
       <c r="E50" s="4">
-        <v>701</v>
+        <v>185</v>
       </c>
       <c r="F50" s="12">
-        <v>706</v>
+        <v>168</v>
       </c>
       <c r="G50" s="4">
-        <v>655</v>
+        <v>156</v>
       </c>
       <c r="H50" s="12">
-        <v>734</v>
+        <v>194</v>
       </c>
       <c r="I50" s="4">
-        <v>719</v>
+        <v>186</v>
       </c>
       <c r="J50" s="12">
-        <v>654</v>
+        <v>165</v>
       </c>
       <c r="K50" s="4">
-        <v>622</v>
+        <v>165</v>
       </c>
       <c r="L50" s="12">
-        <v>640</v>
+        <v>158</v>
       </c>
       <c r="M50" s="4">
-        <v>634</v>
+        <v>178</v>
       </c>
     </row>
     <row r="51" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B51" s="12">
-        <v>214</v>
+        <v>468</v>
       </c>
       <c r="C51" s="4">
-        <v>200</v>
+        <v>499</v>
       </c>
       <c r="D51" s="12">
-        <v>173</v>
+        <v>432</v>
       </c>
       <c r="E51" s="4">
-        <v>185</v>
+        <v>437</v>
       </c>
       <c r="F51" s="12">
-        <v>168</v>
+        <v>455</v>
       </c>
       <c r="G51" s="4">
-        <v>156</v>
+        <v>430</v>
       </c>
       <c r="H51" s="12">
-        <v>194</v>
+        <v>440</v>
       </c>
       <c r="I51" s="4">
-        <v>186</v>
+        <v>461</v>
       </c>
       <c r="J51" s="12">
-        <v>165</v>
+        <v>401</v>
       </c>
       <c r="K51" s="4">
-        <v>165</v>
+        <v>411</v>
       </c>
       <c r="L51" s="12">
-        <v>158</v>
+        <v>380</v>
       </c>
       <c r="M51" s="4">
-        <v>178</v>
+        <v>405</v>
       </c>
     </row>
     <row r="52" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B52" s="12">
-        <v>468</v>
+        <v>1029</v>
       </c>
       <c r="C52" s="4">
-        <v>499</v>
+        <v>982</v>
       </c>
       <c r="D52" s="12">
-        <v>432</v>
+        <v>959</v>
       </c>
       <c r="E52" s="4">
-        <v>437</v>
+        <v>929</v>
       </c>
       <c r="F52" s="12">
-        <v>455</v>
+        <v>976</v>
       </c>
       <c r="G52" s="4">
-        <v>430</v>
+        <v>941</v>
       </c>
       <c r="H52" s="12">
-        <v>440</v>
+        <v>924</v>
       </c>
       <c r="I52" s="4">
-        <v>461</v>
+        <v>951</v>
       </c>
       <c r="J52" s="12">
-        <v>401</v>
+        <v>911</v>
       </c>
       <c r="K52" s="4">
-        <v>411</v>
+        <v>878</v>
       </c>
       <c r="L52" s="12">
-        <v>380</v>
+        <v>917</v>
       </c>
       <c r="M52" s="4">
-        <v>405</v>
+        <v>887</v>
       </c>
     </row>
     <row r="53" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B53" s="12">
-        <v>1029</v>
+        <v>415</v>
       </c>
       <c r="C53" s="4">
-        <v>982</v>
+        <v>409</v>
       </c>
       <c r="D53" s="12">
-        <v>959</v>
+        <v>389</v>
       </c>
       <c r="E53" s="4">
-        <v>929</v>
+        <v>383</v>
       </c>
       <c r="F53" s="12">
-        <v>976</v>
+        <v>400</v>
       </c>
       <c r="G53" s="4">
-        <v>941</v>
+        <v>370</v>
       </c>
       <c r="H53" s="12">
-        <v>924</v>
+        <v>393</v>
       </c>
       <c r="I53" s="4">
-        <v>951</v>
+        <v>355</v>
       </c>
       <c r="J53" s="12">
-        <v>911</v>
+        <v>378</v>
       </c>
       <c r="K53" s="4">
-        <v>878</v>
+        <v>362</v>
       </c>
       <c r="L53" s="12">
-        <v>917</v>
+        <v>349</v>
       </c>
       <c r="M53" s="4">
-        <v>887</v>
+        <v>333</v>
       </c>
     </row>
     <row r="54" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -14171,6 +14170,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -14181,7 +14181,9 @@
   </sheetPr>
   <dimension ref="A1:M80"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A53" sqref="A53:M53"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -17471,6 +17473,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -17481,7 +17484,9 @@
   </sheetPr>
   <dimension ref="A1:M80"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N2" sqref="N2:N80"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -20781,7 +20786,9 @@
   </sheetPr>
   <dimension ref="A1:M80"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A52" sqref="A52"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -24081,7 +24088,9 @@
   </sheetPr>
   <dimension ref="A1:M80"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="A53" sqref="A53"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>